<commit_message>
BOM and datasheet cleanup for V0.1
</commit_message>
<xml_diff>
--- a/Electronic Design/Interactive Core Memory Badge v0.1/Interactive Core Memory Badge v0.1 BOM.xlsx
+++ b/Electronic Design/Interactive Core Memory Badge v0.1/Interactive Core Memory Badge v0.1 BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/OneDrive/00_MBP2011-Documents/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/Interactive Core Memory Badge v0.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{5ECBB0A8-F159-2B47-B487-F3CAA18A3F33}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{77E64577-295E-F84A-9E05-40F7CB1AE767}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{5ECBB0A8-F159-2B47-B487-F3CAA18A3F33}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{0A0AC661-EC2B-2746-9D29-853D36491B1E}"/>
   <bookViews>
     <workbookView xWindow="5160" yWindow="-28340" windowWidth="27640" windowHeight="21700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1447,8 +1447,8 @@
   </sheetPr>
   <dimension ref="A1:P127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3933,7 +3933,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:16" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>11</v>
       </c>

</xml_diff>